<commit_message>
code update (Oct, 2021)
</commit_message>
<xml_diff>
--- a/data/Stockyard_area.xlsx
+++ b/data/Stockyard_area.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nam Sohyun\PycharmProjects\KSOE-Layout\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohyon\PycharmProjects\Simulation_Module\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77C6BFC-8714-42F0-ADBD-4A0C5C80740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7325897-890E-4E65-AF5A-D4402E60852B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFE457C6-1D06-4652-B872-6C32EF543325}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12204" xr2:uid="{FFE457C6-1D06-4652-B872-6C32EF543325}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>E4</t>
   </si>
@@ -81,11 +81,19 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>Stock</t>
+    <t>area</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>area</t>
+    <t>Y9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y80</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -452,20 +460,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528D6D40-B1E4-45E7-9AD0-17A660D455BC}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -586,6 +594,22 @@
       </c>
       <c r="B16" s="2">
         <v>11267.228926600001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>22681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>